<commit_message>
Modification des fichiers sur le rapport d'optimisation
</commit_message>
<xml_diff>
--- a/Rapport optimisation/audit-SEO.xlsx
+++ b/Rapport optimisation/audit-SEO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Catégorie</t>
   </si>
@@ -36,85 +36,79 @@
     <t>Référence</t>
   </si>
   <si>
+    <t>Optimisé</t>
+  </si>
+  <si>
+    <t>SEO et accessibilité</t>
+  </si>
+  <si>
+    <t>Balise Meta et attribut Lang</t>
+  </si>
+  <si>
+    <t>Les balises sont présentes dans le fichier HTML, mais elles ne sont pas exploitées.</t>
+  </si>
+  <si>
+    <t>Il faut ajouter les mots-clés, et décrire le contenu de chaque page.</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Balise Meta</t>
+  </si>
+  <si>
+    <t>La balise Meta Keywords a plusieurs fois le même mot-clé.</t>
+  </si>
+  <si>
+    <t>La balise meta Keywords doit avoir au maximum 10 mots-clés.</t>
+  </si>
+  <si>
+    <t>Balise Meta Keywords</t>
+  </si>
+  <si>
+    <t>L'attribut Lang à la valeur "default".</t>
+  </si>
+  <si>
+    <t>Il faut mettre la langue adaptée au contenu.</t>
+  </si>
+  <si>
+    <t>Le code source de chaque page indique la langue principale du contenu.</t>
+  </si>
+  <si>
+    <t>SEO et accesibilité</t>
+  </si>
+  <si>
+    <t>Balise sémantique</t>
+  </si>
+  <si>
+    <t>Les fichiers HTML utilisent des div au lieu des balises sémantiques.</t>
+  </si>
+  <si>
+    <t>Il faut utiliser les balises adaptées à son contenu.</t>
+  </si>
+  <si>
+    <t>Barre de navigation</t>
+  </si>
+  <si>
+    <t>La barre de navigation contient le lien "page 2 &gt;" qui ne précisent pas, vers quel contenu l'utilisateur sera redirigé.</t>
+  </si>
+  <si>
+    <t>Il faut au lien un libellé plus explicite sur le contenu qu'il redirige.</t>
+  </si>
+  <si>
+    <t>Chaque lien est doté d'un intitulé dans le code source.</t>
+  </si>
+  <si>
     <t>SEO</t>
   </si>
   <si>
-    <t>Balise Title et description.</t>
-  </si>
-  <si>
-    <t>Les balise sont présente dans le fichier html, mais elle ne sont pas exploité.</t>
-  </si>
-  <si>
-    <t>Il faut ajouter les mots-clés, et décrire le contenu de châque page.</t>
-  </si>
-  <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>Checklist Opquast numéro 45, 46, 48, 49, 50 et 52.</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>SEO et accesibilité</t>
-  </si>
-  <si>
-    <t>Les balises sémantiques.</t>
-  </si>
-  <si>
-    <t>Les fichiers html utilisent des div au lieu des balises sémantiques.</t>
-  </si>
-  <si>
-    <t>Il faut utiliser les balises adapté à son contenu.</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/fr/docs/Apprendre/a11y/HTML</t>
-  </si>
-  <si>
-    <t>Meta keywords</t>
-  </si>
-  <si>
-    <t>La balise Meta keywords a plusieurs fois le même mot-clé.</t>
-  </si>
-  <si>
-    <t>La balise meta keywords doit avoir au maximun 10 mots clés.</t>
-  </si>
-  <si>
-    <t>Checklist Opquast numéro 43 et 44.</t>
-  </si>
-  <si>
-    <t>Attribut lang</t>
-  </si>
-  <si>
-    <t>L'attribut lang à la valeur "default".</t>
-  </si>
-  <si>
-    <t>Il faut mettre la langue adapté au contenu.</t>
-  </si>
-  <si>
-    <t>Checklist Opquast numéro 7.</t>
-  </si>
-  <si>
-    <t>Barre de navigation</t>
-  </si>
-  <si>
-    <t>La barre de navigation contient le lien "page 2 &gt;" qui ne précise pas, vers quelle contenu l'utilisateur sera redirigé.</t>
-  </si>
-  <si>
-    <t>Il faut au lien un libéllé plus explicite sur le contenu qu'il redirige.</t>
-  </si>
-  <si>
-    <t>Checklist Opquast numéro 131.</t>
-  </si>
-  <si>
-    <t>Mot clés caché.</t>
-  </si>
-  <si>
-    <t>On retrouve dans les fichiers HTML, des mots clés cachés. Cette pratique est mauvaise pour le référencement car elle est bannit par google.</t>
-  </si>
-  <si>
-    <t>Il faut retirer et éviter de cacher les mots clés.</t>
+    <t>Mot clé caché.</t>
+  </si>
+  <si>
+    <t>On retrouve dans les fichiers HTML, des mots-clés cachés. Cette pratique est mauvaise pour le référencement car elle est bannie par google.</t>
+  </si>
+  <si>
+    <t>Il faut retirer et éviter de cacher les mots-clés.</t>
   </si>
   <si>
     <t>Texte caché</t>
@@ -126,19 +120,19 @@
     <t>Le texte alternatif ne donne pas une description adaptée à l'image.</t>
   </si>
   <si>
-    <t>Il faut que chaque image ait sont texte alternatifs approprié.</t>
-  </si>
-  <si>
-    <t>Opquast n°113</t>
-  </si>
-  <si>
-    <t>Image utilisé pour ajouter du texte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le site contient des images avec du texte, cette pratique empêche les robots d'accéder au contenu, et nuie à l'accesibilité. </t>
-  </si>
-  <si>
-    <t>Il faut priviligié l'utilisation des balises pour afficher le texte.</t>
+    <t>Il faut que chaque image ait son texte alternatif approprié.</t>
+  </si>
+  <si>
+    <t>Les images porteuses d'informations</t>
+  </si>
+  <si>
+    <t>Image utilisée pour ajouter du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le site contient des images avec du texte, cette pratique empêche les robots d'accéder au contenu, et nui à l'accessibilité. </t>
+  </si>
+  <si>
+    <t>Il faut privilégier l'utilisation des balises pour afficher le texte.</t>
   </si>
   <si>
     <t>Éviter les images avec du texte</t>
@@ -147,10 +141,10 @@
     <t xml:space="preserve">Texte et couleur </t>
   </si>
   <si>
-    <t>Plusieurs paragraphes sont trop petit et ont une couleur qui ne convient pas pour la lecture.</t>
-  </si>
-  <si>
-    <t>Il est recommandé d'avoir une taille de police entre 10 et 12 points. Il faut également conservé un contraste minimal de 3:1 entre le texte et son arrière-plan.</t>
+    <t>Plusieurs paragraphes sont trop petits et ont une couleur qui ne convient pas pour la lecture.</t>
+  </si>
+  <si>
+    <t>Il est recommandé d'avoir une taille de police entre 10 et 12 points. Il faut également conserver un contraste minimal de 3:1 entre le texte et son arrière-plan.</t>
   </si>
   <si>
     <r>
@@ -163,6 +157,7 @@
     <r>
       <rPr>
         <color rgb="FF000000"/>
+        <u/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -175,13 +170,13 @@
     </r>
   </si>
   <si>
-    <t>Liens mort</t>
-  </si>
-  <si>
-    <t>Il y a tout une liste de liens dans le footer qui ne marche pas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un trop grand nombre de lien mort baisse la pertinence du site pour les robots de google, ce qui peut diminuer le traffic et baisser le classement dans les moteurs de recherches. </t>
+    <t>Liens morts</t>
+  </si>
+  <si>
+    <t>Il y a toute une liste de liens dans le footer qui ne marche pas.</t>
+  </si>
+  <si>
+    <t>Un trop grand nombre de liens mort, ce qui peut nuire à la pertinence du site pour les robots de google, ce qui peut diminuer le trafic et baisser le classement dans les moteurs de recherche.</t>
   </si>
   <si>
     <t>Non</t>
@@ -193,20 +188,80 @@
     <t>Design</t>
   </si>
   <si>
-    <t>Le design du site manque de cohérence graphique, en exemple la page de contact n'a pas de photo en arrière plan avec un effet parallaxe.</t>
+    <t>Le design du site manque de cohérence graphique, en exemple la page de contact n'a pas de photo en arrière-plan avec un effet parallaxe.</t>
   </si>
   <si>
     <t>Appliquer le même style pour toute les pages.</t>
   </si>
   <si>
     <t>Charte graphique</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>CSS minifié</t>
+  </si>
+  <si>
+    <t>Le fichier style.css n'a pas était minifier.</t>
+  </si>
+  <si>
+    <t>Il faut faire une copie du fichier CSS pour le minifier et changer le lien du fichier dans la balise link.</t>
+  </si>
+  <si>
+    <t>CSS minifier</t>
+  </si>
+  <si>
+    <t>Optimisations des images</t>
+  </si>
+  <si>
+    <t>Les images n'utilisent pas le bon format et ne sont pas compressées</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Changer les images qui sont au format </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>bmp</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> vers le format </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+      </rPr>
+      <t>. Compresser les images avec un outil en ligne.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -221,10 +276,10 @@
     <font>
       <b/>
       <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FFFFFFFF"/>
     </font>
     <font>
+      <b/>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -237,6 +292,11 @@
     <font>
       <u/>
       <color rgb="FF1155CC"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -265,40 +325,43 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
@@ -308,6 +371,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,7 +604,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -550,310 +616,318 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" ht="65.25" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="G2" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="49.5" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" ht="49.5" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="8" t="s">
+    </row>
+    <row r="5" ht="49.5" customHeight="1">
+      <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="36.75" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>12</v>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="77.25" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="G6" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="90.75" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" ht="72.0" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>12</v>
+      <c r="G7" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="51.0" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>12</v>
+      <c r="G8" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" ht="85.5" customHeight="1">
-      <c r="A9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>12</v>
+      <c r="G9" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="99.0" customHeight="1">
-      <c r="A10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>12</v>
+      <c r="G10" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="105.0" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="F11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="G11" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="88.5" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="D12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" ht="81.0" customHeight="1">
-      <c r="A12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="8" t="s">
+    <row r="13" ht="60.0" customHeight="1">
+      <c r="A13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>12</v>
+      <c r="C13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="11"/>
+    <row r="14" ht="80.25" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="11"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -1841,18 +1915,29 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="G2:G4"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F3"/>
-    <hyperlink r:id="rId2" ref="F7"/>
-    <hyperlink r:id="rId3" ref="F8"/>
-    <hyperlink r:id="rId4" location=":~:text=%C3%89vitez%20les%20images%20avec%20du,%C3%80%20%C3%A9viter%20!" ref="F9"/>
-    <hyperlink r:id="rId5" ref="F10"/>
-    <hyperlink r:id="rId6" ref="F11"/>
-    <hyperlink r:id="rId7" ref="F12"/>
+    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink r:id="rId2" ref="F3"/>
+    <hyperlink r:id="rId3" ref="F4"/>
+    <hyperlink r:id="rId4" ref="F5"/>
+    <hyperlink r:id="rId5" ref="F6"/>
+    <hyperlink r:id="rId6" ref="F7"/>
+    <hyperlink r:id="rId7" ref="F8"/>
+    <hyperlink r:id="rId8" location=":~:text=%C3%89vitez%20les%20images%20avec%20du,%C3%80%20%C3%A9viter%20!" ref="F9"/>
+    <hyperlink r:id="rId9" ref="F10"/>
+    <hyperlink r:id="rId10" ref="F11"/>
+    <hyperlink r:id="rId11" ref="F12"/>
+    <hyperlink r:id="rId12" ref="F13"/>
+    <hyperlink r:id="rId13" location=":~:text=L'optimisation%20des%20images%20est,sont%20deux%20m%C3%A9thodes%20couramment%20utilis%C3%A9es." ref="F14"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>